<commit_message>
Optimization Success | :( memory leaks
</commit_message>
<xml_diff>
--- a/time_optimization.xlsx
+++ b/time_optimization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Others\source\repos\Chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E159783E-EA1C-4B89-95DC-238E5C56B37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4418466-50E3-46AC-9647-C7410C4C26E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{57897172-06F5-4A42-8E47-4E3B3D7B28DC}"/>
+    <workbookView xWindow="2760" yWindow="3375" windowWidth="21600" windowHeight="11295" xr2:uid="{57897172-06F5-4A42-8E47-4E3B3D7B28DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>AVG_VECTOR_C</t>
   </si>
   <si>
     <t>AVG_VECTOR_GPU_FIRST_ATT</t>
+  </si>
+  <si>
+    <t>GPU_Ndimentions method</t>
+  </si>
+  <si>
+    <t>GPU_GENERATIVE</t>
   </si>
 </sst>
 </file>
@@ -140,31 +146,83 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-EE1B-4CC7-A71A-FEC6D1215751}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-EE1B-4CC7-A71A-FEC6D1215751}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$C$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>AVG_VECTOR_C</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>AVG_VECTOR_GPU_FIRST_ATT</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>GPU_Ndimentions method</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>GPU_GENERATIVE</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$C$10</c:f>
+              <c:f>Sheet1!$B$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.4485749999999994E-2</c:v>
+                  <c:v>6.3977999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0693539999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2021930000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5343000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,16 +952,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1228,73 +1286,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073E14B9-49E0-4509-AACD-34048F0ED170}">
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>6.1549E-2</v>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>6.8481E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>6.3033000000000006E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>6.6747000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>6.2273000000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>6.6392000000000007E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>6.3977999999999993E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>6.3433000000000003E-2</v>
+      <c r="C2">
+        <v>1.0693539999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <f>AVERAGE(B2:B9)</f>
-        <v>6.4485749999999994E-2</v>
+      <c r="D2">
+        <v>1.2021930000000001</v>
       </c>
-      <c r="C10">
-        <v>1.0693539999999999</v>
+      <c r="E2">
+        <v>4.5343000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Matrix Mul For HIdden Layer BackProbagation
Result not verified as correct.
</commit_message>
<xml_diff>
--- a/time_optimization.xlsx
+++ b/time_optimization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Others\source\repos\Chess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3DCCF0-4532-4A37-A135-AE1201FF9BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3109723F-51D4-4662-B4CC-902CBCC207EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="3375" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{57897172-06F5-4A42-8E47-4E3B3D7B28DC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>AVG_VECTOR_C</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>FIRST_ATTEMPT</t>
+  </si>
+  <si>
+    <t>MATRIX_MUL</t>
   </si>
 </sst>
 </file>
@@ -530,31 +533,58 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-AF8E-45C5-9DDA-0DC652F8118E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>BACK_PROP!$B$1:$C$1</c:f>
+              <c:f>BACK_PROP!$B$1:$D$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>SEQUANTIAL</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>FIRST_ATTEMPT</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>MATRIX_MUL</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BACK_PROP!$B$2:$C$2</c:f>
+              <c:f>BACK_PROP!$B$2:$D$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2276,13 +2306,14 @@
   <dimension ref="B1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2293,6 +2324,9 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -2300,6 +2334,9 @@
       </c>
       <c r="C2">
         <v>1096</v>
+      </c>
+      <c r="D2">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>